<commit_message>
fixes to lifemap decisions for vendor_set
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/prospec.xlsx
+++ b/rufus/carriers/lifemap_science/order/prospec.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="2060" yWindow="0" windowWidth="34980" windowHeight="20800" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3_prospec.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -51,12 +51,6 @@
     <t>out:Handling Fee</t>
   </si>
   <si>
-    <t>in:vendor</t>
-  </si>
-  <si>
-    <t>ProSpec</t>
-  </si>
-  <si>
     <t>&gt;6</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>FedEx NextDay Styrofoam Box</t>
+  </si>
+  <si>
+    <t>in:vendor_set</t>
+  </si>
+  <si>
+    <t>$(ProSpec)</t>
   </si>
 </sst>
 </file>
@@ -164,8 +164,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -262,7 +264,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -306,6 +308,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -349,6 +352,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,39 +685,39 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="64.5" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" customWidth="1"/>
     <col min="5" max="6" width="19.5" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
@@ -736,19 +740,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2000</v>
@@ -771,19 +775,19 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
       <c r="F4">
         <v>2000</v>
@@ -806,19 +810,19 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
       </c>
       <c r="F5">
         <v>2000</v>
@@ -832,11 +836,11 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" t="s">
-        <v>11</v>
+      <c r="A6" t="s">
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>4500</v>
@@ -855,11 +859,11 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="C7" t="s">
-        <v>11</v>
+      <c r="A7" t="s">
+        <v>20</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5">
         <v>5500</v>

</xml_diff>

<commit_message>
need to use to_rudelo and from_rudelo
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/prospec.xlsx
+++ b/rufus/carriers/lifemap_science/order/prospec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="12740" windowWidth="32760" windowHeight="7360" tabRatio="500"/>
+    <workbookView xWindow="-38360" yWindow="11060" windowWidth="38360" windowHeight="8760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="3_prospec.csv" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,6 @@
     <t>in:total_order_price</t>
   </si>
   <si>
-    <t>$(Recombinant protein) intersection $in #=0</t>
-  </si>
-  <si>
-    <t>$in &gt;= $(Recombinant protein)</t>
-  </si>
-  <si>
     <t>&lt;2500.01</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>$in &gt;= $(ice_packs)</t>
+  </si>
+  <si>
+    <t>$(ice-packs) intersection $in #=0</t>
   </si>
 </sst>
 </file>
@@ -179,8 +179,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -293,7 +297,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -345,6 +349,8 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -396,6 +402,8 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,7 +736,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -790,13 +798,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -828,13 +836,13 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -866,7 +874,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -901,13 +909,13 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -922,16 +930,16 @@
         <v>8500</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -939,7 +947,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -965,7 +973,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
update rules for prospec
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/prospec.xlsx
+++ b/rufus/carriers/lifemap_science/order/prospec.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38000" yWindow="1360" windowWidth="38360" windowHeight="8760" tabRatio="500"/>
+    <workbookView xWindow="6980" yWindow="0" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="3_prospec.csv" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>accumulate</t>
   </si>
   <si>
-    <t>&gt;6</t>
-  </si>
-  <si>
     <t>out:Package</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>&lt;2500.01</t>
   </si>
   <si>
-    <t>&gt;2500.00</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -97,6 +91,9 @@
   </si>
   <si>
     <t>out:FedExZone 3</t>
+  </si>
+  <si>
+    <t>lyophilized freeze-dry</t>
   </si>
 </sst>
 </file>
@@ -761,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,60 +786,60 @@
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>2000</v>
@@ -865,171 +862,116 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>2000</v>
       </c>
       <c r="H4" s="5">
-        <v>12000</v>
-      </c>
-      <c r="I4" s="5">
-        <v>13000</v>
-      </c>
-      <c r="J4" s="5">
-        <v>17500</v>
-      </c>
-      <c r="K4" s="5">
-        <v>17500</v>
-      </c>
-      <c r="L4" s="5">
-        <v>25000</v>
+        <v>8500</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>2000</v>
-      </c>
-      <c r="H5" s="5">
-        <v>12000</v>
-      </c>
-      <c r="I5" s="5">
-        <v>13000</v>
-      </c>
-      <c r="J5" s="5">
-        <v>17500</v>
-      </c>
-      <c r="K5" s="5">
-        <v>17500</v>
-      </c>
-      <c r="L5" s="5">
-        <v>25000</v>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4500</v>
+      </c>
+      <c r="I5">
+        <v>5500</v>
+      </c>
+      <c r="J5">
+        <v>6500</v>
+      </c>
+      <c r="K5">
+        <v>6000</v>
+      </c>
+      <c r="L5">
+        <v>8000</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5500</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>2000</v>
-      </c>
-      <c r="H6" s="5">
-        <v>8500</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>4500</v>
-      </c>
-      <c r="I7">
-        <v>5500</v>
-      </c>
-      <c r="J7">
-        <v>6500</v>
-      </c>
-      <c r="K7">
-        <v>6000</v>
-      </c>
-      <c r="L7">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>5500</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert rule change manually
</commit_message>
<xml_diff>
--- a/rufus/carriers/lifemap_science/order/prospec.xlsx
+++ b/rufus/carriers/lifemap_science/order/prospec.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="0" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="-38000" yWindow="1360" windowWidth="38360" windowHeight="8760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="3_prospec.csv" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>accumulate</t>
   </si>
   <si>
+    <t>&gt;6</t>
+  </si>
+  <si>
     <t>out:Package</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
     <t>&lt;2500.01</t>
   </si>
   <si>
+    <t>&gt;2500.00</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -91,9 +97,6 @@
   </si>
   <si>
     <t>out:FedExZone 3</t>
-  </si>
-  <si>
-    <t>lyophilized freeze-dry</t>
   </si>
 </sst>
 </file>
@@ -758,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -786,60 +789,60 @@
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
       </c>
       <c r="G3">
         <v>2000</v>
@@ -862,116 +865,171 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
       </c>
       <c r="G4">
         <v>2000</v>
       </c>
       <c r="H4" s="5">
-        <v>8500</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>10</v>
+        <v>12000</v>
+      </c>
+      <c r="I4" s="5">
+        <v>13000</v>
+      </c>
+      <c r="J4" s="5">
+        <v>17500</v>
+      </c>
+      <c r="K4" s="5">
+        <v>17500</v>
+      </c>
+      <c r="L4" s="5">
+        <v>25000</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>4500</v>
-      </c>
-      <c r="I5">
-        <v>5500</v>
-      </c>
-      <c r="J5">
-        <v>6500</v>
-      </c>
-      <c r="K5">
-        <v>6000</v>
-      </c>
-      <c r="L5">
-        <v>8000</v>
+        <v>2000</v>
+      </c>
+      <c r="H5" s="5">
+        <v>12000</v>
+      </c>
+      <c r="I5" s="5">
+        <v>13000</v>
+      </c>
+      <c r="J5" s="5">
+        <v>17500</v>
+      </c>
+      <c r="K5" s="5">
+        <v>17500</v>
+      </c>
+      <c r="L5" s="5">
+        <v>25000</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
       <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="5">
+        <v>8500</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H7">
+        <v>4500</v>
+      </c>
+      <c r="I7">
         <v>5500</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>10</v>
+      <c r="J7">
+        <v>6500</v>
+      </c>
+      <c r="K7">
+        <v>6000</v>
+      </c>
+      <c r="L7">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>5500</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>